<commit_message>
Haarlemmer meer was misspelled causing errors
</commit_message>
<xml_diff>
--- a/Data_files/Part_1/Randstad_ov_adjacency.xlsx
+++ b/Data_files/Part_1/Randstad_ov_adjacency.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tud365.sharepoint.com/sites/DesigninNetwork/Gedeelde documenten/General/Excel and CSV files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimEW\PycharmProjects\Design_in_Network_group_8\Data_files\Part_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="11_8D2383B83A8F73713B5DD365A3B46C6327ED40E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A32B6B53-67B7-44C0-8DF1-3E7DEC6F8D1E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EFB0A2F-B691-45DF-8B38-DD96321C53D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -101,9 +101,6 @@
     <t>Schiedam</t>
   </si>
   <si>
-    <t>Schiphol Haarlemermeer</t>
-  </si>
-  <si>
     <t>Locations</t>
   </si>
   <si>
@@ -117,6 +114,9 @@
   </si>
   <si>
     <t>Longitude</t>
+  </si>
+  <si>
+    <t>Schiphol Haarlemmermeer</t>
   </si>
 </sst>
 </file>
@@ -521,22 +521,25 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.81640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="F1" s="1">
         <v>0</v>
@@ -1686,7 +1689,7 @@
     </row>
     <row r="15" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B15" s="1">
         <v>162300</v>
@@ -2437,18 +2440,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2596,14 +2599,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEEA0459-F893-458F-A568-7B18BE0C703B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{918F29E8-6AAD-4178-A843-74E1D3B2E11F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -2615,6 +2610,14 @@
     <ds:schemaRef ds:uri="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEEA0459-F893-458F-A568-7B18BE0C703B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
restarted kernel and ran everything 2 plus some bug fixes in the travel time minimise function
</commit_message>
<xml_diff>
--- a/Data_files/Part_1/Randstad_ov_adjacency.xlsx
+++ b/Data_files/Part_1/Randstad_ov_adjacency.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimEW\PycharmProjects\Design_in_Network_group_8\Data_files\Part_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EFB0A2F-B691-45DF-8B38-DD96321C53D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BCE5711-CA35-41D4-BE16-6CD949F223E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,9 +54,6 @@
   </si>
   <si>
     <t>Delft</t>
-  </si>
-  <si>
-    <t>Den Haag </t>
   </si>
   <si>
     <t>Dordrecht</t>
@@ -117,6 +114,9 @@
   </si>
   <si>
     <t>Schiphol Haarlemmermeer</t>
+  </si>
+  <si>
+    <t>Den Haag</t>
   </si>
 </sst>
 </file>
@@ -517,7 +517,7 @@
   <dimension ref="A1:AA23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -527,19 +527,19 @@
   <sheetData>
     <row r="1" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="F1" s="1">
         <v>0</v>
@@ -1108,7 +1108,7 @@
     </row>
     <row r="8" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="B8" s="1">
         <v>562839</v>
@@ -1191,7 +1191,7 @@
     </row>
     <row r="9" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="1">
         <v>121434</v>
@@ -1274,7 +1274,7 @@
     </row>
     <row r="10" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="1">
         <v>75316</v>
@@ -1357,7 +1357,7 @@
     </row>
     <row r="11" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="1">
         <v>165396</v>
@@ -1440,7 +1440,7 @@
     </row>
     <row r="12" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="1">
         <v>93345</v>
@@ -1523,7 +1523,7 @@
     </row>
     <row r="13" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="1">
         <v>127089</v>
@@ -1606,7 +1606,7 @@
     </row>
     <row r="14" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" s="1">
         <v>663900</v>
@@ -1689,7 +1689,7 @@
     </row>
     <row r="15" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" s="1">
         <v>162300</v>
@@ -1772,7 +1772,7 @@
     </row>
     <row r="16" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="1">
         <v>72561</v>
@@ -1855,7 +1855,7 @@
     </row>
     <row r="17" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B17" s="1">
         <v>367947</v>
@@ -1938,7 +1938,7 @@
     </row>
     <row r="18" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="1">
         <v>75079</v>
@@ -2021,7 +2021,7 @@
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="1">
         <v>114887</v>
@@ -2104,7 +2104,7 @@
     </row>
     <row r="20" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" s="1">
         <v>53244</v>
@@ -2187,7 +2187,7 @@
     </row>
     <row r="21" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21" s="1">
         <v>159618</v>
@@ -2270,7 +2270,7 @@
     </row>
     <row r="22" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" s="1">
         <v>126998</v>
@@ -2353,7 +2353,7 @@
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23" s="1">
         <v>77999</v>

</xml_diff>